<commit_message>
added EfromDev automate testScenario
</commit_message>
<xml_diff>
--- a/ExcelFileData/WriteItemData.xlsx
+++ b/ExcelFileData/WriteItemData.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
   <si>
     <t>boAt Airdopes 121v2 On Ear True Wireless (TWS) 14 Hours Playback IPX7(Water Resistant) Active Noise cancellation -Bluetooth V 5.0 Black</t>
   </si>
@@ -29,13 +29,7 @@
     <t>NBOX STAR 40 HOURS MUSIC PLAYBACK WIRELESS NECKBAND WITH DOLBY EFFECT BASS SOUND IPX5 WITH MASSIVE MUSIC PLAYBACK,BLUETOOTH HEADPHONE,BLUETOOTH EARPHONE FOR NBOX</t>
   </si>
   <si>
-    <t>Rs. 700</t>
-  </si>
-  <si>
-    <t>NBOX INVICTUS Neckband Wireless With Mic Headphones/Earphones Multicolor</t>
-  </si>
-  <si>
-    <t>Rs. 899</t>
+    <t>NBOX STAR WIRELESS NECKBAND WITH DOLBY EFFECT BASS SOUND IPX5 WITH MASSIVE MUSIC PLAYBACK WITH 1 YEAR WARRANTY BLUETOOTH HEADPHONE,BLUETOOTH EARPHONE,BLUETOOTH NECKBAND</t>
   </si>
   <si>
     <t>boAt Airdopes 131/138 Twin Wireless Earbuds with IWP Technology, Bluetooth V5.0, Immersive Audio, Up to 15H Total Playback, Instant Voice Assistant and Type-C Charging,Bluetooth Earphone (Active Black)</t>
@@ -110,20 +104,20 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
data provider with Excel
</commit_message>
<xml_diff>
--- a/ExcelFileData/WriteItemData.xlsx
+++ b/ExcelFileData/WriteItemData.xlsx
@@ -12,27 +12,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
-    <t>boAt Airdopes 121v2 On Ear True Wireless (TWS) 14 Hours Playback IPX7(Water Resistant) Active Noise cancellation -Bluetooth V 5.0 Black</t>
+    <t>boAt Airdopes 131/138 Twin Wireless Earbuds with IWP Technology, Bluetooth V5.0, Immersive Audio, Up to 15H Total Playback, Instant Voice Assistant and Type-C Charging,Bluetooth Earphone (Active Black)</t>
   </si>
   <si>
     <t>Rs. 1,299</t>
   </si>
   <si>
-    <t>NBOX MARATHON 20 HOURS MUSIC PLAYBACK IPX4 4D BASS SPORT Bluetooth headphone / Bluetooth earphone Magnetic bluetooth neckband - Silver</t>
+    <t>NBOX MARATHON Over Ear Bluetooth Neckband 20 Hours Playback IPX5(Splash &amp; Sweat Proof) Passive noise cancellation -Bluetooth Silver</t>
   </si>
   <si>
     <t>Rs. 749</t>
   </si>
   <si>
+    <t>NBOX Air1 TWS On Ear True Wireless (TWS) 20 Hours Playback IPX5(Splash &amp; Sweat Proof) Passive noise cancellation -Bluetooth Black</t>
+  </si>
+  <si>
     <t>NBOX STAR 40 HOURS MUSIC PLAYBACK WIRELESS NECKBAND WITH DOLBY EFFECT BASS SOUND IPX5 WITH MASSIVE MUSIC PLAYBACK,BLUETOOTH HEADPHONE,BLUETOOTH EARPHONE FOR NBOX</t>
   </si>
   <si>
-    <t>NBOX STAR WIRELESS NECKBAND WITH DOLBY EFFECT BASS SOUND IPX5 WITH MASSIVE MUSIC PLAYBACK WITH 1 YEAR WARRANTY BLUETOOTH HEADPHONE,BLUETOOTH EARPHONE,BLUETOOTH NECKBAND</t>
+    <t>Rs. 700</t>
   </si>
   <si>
-    <t>boAt Airdopes 131/138 Twin Wireless Earbuds with IWP Technology, Bluetooth V5.0, Immersive Audio, Up to 15H Total Playback, Instant Voice Assistant and Type-C Charging,Bluetooth Earphone (Active Black)</t>
+    <t>boAt Airdopes 121v2 On Ear True Wireless (TWS) 14 Hours Playback IPX7(Water Resistant) Active Noise cancellation -Bluetooth V 5.0 Black</t>
   </si>
 </sst>
 </file>
@@ -112,12 +115,12 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
FluentWait & additionSiftwareRequest scenario
</commit_message>
<xml_diff>
--- a/ExcelFileData/WriteItemData.xlsx
+++ b/ExcelFileData/WriteItemData.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>boAt Airdopes 131/138 Twin Wireless Earbuds with IWP Technology, Bluetooth V5.0, Immersive Audio, Up to 15H Total Playback, Instant Voice Assistant and Type-C Charging,Bluetooth Earphone (Active Black)</t>
   </si>
@@ -20,19 +20,25 @@
     <t>Rs. 1,299</t>
   </si>
   <si>
-    <t>NBOX MARATHON Over Ear Bluetooth Neckband 20 Hours Playback IPX5(Splash &amp; Sweat Proof) Passive noise cancellation -Bluetooth Silver</t>
+    <t>NBOX Air1 TWS On Ear True Wireless (TWS) 20 Hours Playback IPX5(Splash &amp; Sweat Proof) Passive noise cancellation -Bluetooth Black</t>
   </si>
   <si>
     <t>Rs. 749</t>
   </si>
   <si>
-    <t>NBOX Air1 TWS On Ear True Wireless (TWS) 20 Hours Playback IPX5(Splash &amp; Sweat Proof) Passive noise cancellation -Bluetooth Black</t>
-  </si>
-  <si>
-    <t>boAt Airdopes 131/138 Ear Buds Wireless With Mic Headphones/Earphones (Blue)</t>
+    <t>NBOX MARATHON Over Ear Bluetooth Neckband 20 Hours Playback IPX5(Splash &amp; Sweat Proof) Passive noise cancellation -Bluetooth Silver</t>
   </si>
   <si>
     <t>NBOX G2 PLATINUM SERISE Over Ear Bluetooth Neckband 6 Hours Playback IPX5(Splash &amp; Sweat Proof) Passive noise cancellation -Bluetooth Gray</t>
+  </si>
+  <si>
+    <t>Rs. 700</t>
+  </si>
+  <si>
+    <t>boAt Airdopes 171 On Ear Wireless With Mic Headphones/Earphones Black</t>
+  </si>
+  <si>
+    <t>Rs. 1,499</t>
   </si>
 </sst>
 </file>
@@ -112,15 +118,15 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
extent report with RelativePath
</commit_message>
<xml_diff>
--- a/ExcelFileData/WriteItemData.xlsx
+++ b/ExcelFileData/WriteItemData.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>boAt Airdopes 131/138 Twin Wireless Earbuds with IWP Technology, Bluetooth V5.0, Immersive Audio, Up to 15H Total Playback, Instant Voice Assistant and Type-C Charging,Bluetooth Earphone (Active Black)</t>
   </si>
@@ -20,25 +20,22 @@
     <t>Rs. 1,299</t>
   </si>
   <si>
-    <t>NBOX G2 PLATINUM SERISE Over Ear Bluetooth Neckband 6 Hours Playback IPX5(Splash &amp; Sweat Proof) Passive noise cancellation -Bluetooth Gray</t>
+    <t>NBOX MARATHON Over Ear Bluetooth Neckband 20 Hours Playback IPX5(Splash &amp; Sweat Proof) Passive noise cancellation -Bluetooth Silver</t>
   </si>
   <si>
     <t>Rs. 749</t>
   </si>
   <si>
-    <t>NBOX RISE Neckband Wireless With Mic Headphones/Earphones Black</t>
+    <t>NBOX Buzz TWS On Ear True Wireless (TWS) 20 Hours Playback IPX5(Splash &amp; Sweat Proof) Passive noise cancellation -Bluetooth Version 5.1 Black</t>
   </si>
   <si>
-    <t>Rs. 799</t>
+    <t>boAt Airdopes 121v2 On Ear True Wireless (TWS) 14 Hours Playback IPX7(Water Resistant) Active Noise cancellation -Bluetooth V 5.0 Black</t>
   </si>
   <si>
-    <t>NBOX STAR WIRELESS NECKBAND WITH DOLBY EFFECT BASS SOUND IPX5 WITH MASSIVE MUSIC PLAYBACK WITH 1 YEAR WARRANTY BLUETOOTH HEADPHONE,BLUETOOTH EARPHONE,BLUETOOTH NECKBAND</t>
+    <t>VEhop Power Bank Earbuds, On Ear True Wireless (TWS) 280 Hours Playback IPX4(Splash &amp; Sweat Proof) Passive noise cancellation -Bluetooth V 5.2 Black</t>
   </si>
   <si>
-    <t>boAt 103 Wireless Blue Neckband Wireless With Mic Headphones/Earphones Blue</t>
-  </si>
-  <si>
-    <t>Rs. 1,199</t>
+    <t>Rs. 999</t>
   </si>
 </sst>
 </file>
@@ -110,23 +107,23 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new extentreport with logs and ApiBasic Utils
</commit_message>
<xml_diff>
--- a/ExcelFileData/WriteItemData.xlsx
+++ b/ExcelFileData/WriteItemData.xlsx
@@ -12,12 +12,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
-    <t>boAt Airdopes 131/138 Twin Wireless Earbuds with IWP Technology, Bluetooth V5.0, Immersive Audio, Up to 15H Total Playback, Instant Voice Assistant and Type-C Charging,Bluetooth Earphone (Active Black)</t>
+    <t>boAt Airdopes 131/138 Twin Wireless Earbuds with IWP Technology, Bluetooth V5.0, Immersive Audio, Up to 15H Total Playback, Instant Voice Assistant and Type-C Charging,Bluetooth Earphone (Cherry Blossom)</t>
   </si>
   <si>
     <t>Rs. 1,299</t>
+  </si>
+  <si>
+    <t>Boult Audio Y1 In Ear True Wireless (TWS) 40 Hours Playback IPX5(Splash &amp; Sweat Proof) Powerfull bass -Bluetooth White</t>
+  </si>
+  <si>
+    <t>Rs. 1,499</t>
   </si>
   <si>
     <t>NBOX MARATHON Over Ear Bluetooth Neckband 20 Hours Playback IPX5(Splash &amp; Sweat Proof)BT 5.1 V Passive noise cancellation BLUETOOTH HEADPHONE -Bluetooth Silver</t>
@@ -29,13 +35,10 @@
     <t>NBOX Buzz TWS On Ear True Wireless (TWS) 20 Hours Playback IPX5(Splash &amp; Sweat Proof) Passive noise cancellation -Bluetooth Version 5.1 Black</t>
   </si>
   <si>
-    <t>boAt Airdopes 121v2 On Ear True Wireless (TWS) 14 Hours Playback IPX7(Water Resistant) Active Noise cancellation -Bluetooth V 5.0 Black</t>
+    <t>Varni Airgo In Ear Bluetooth Earphone Hours Playback Bluetooth IPX5(Splash Proof) Active Noise cancellation -Bluetooth White</t>
   </si>
   <si>
-    <t>Zebronics - Wireless Bluetooth Headset</t>
-  </si>
-  <si>
-    <t>Rs. 1,399</t>
+    <t>Rs. 849</t>
   </si>
 </sst>
 </file>
@@ -107,23 +110,23 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new extent report with logs
</commit_message>
<xml_diff>
--- a/ExcelFileData/WriteItemData.xlsx
+++ b/ExcelFileData/WriteItemData.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>boAt Airdopes 131/138 Twin Wireless Earbuds with IWP Technology, Bluetooth V5.0, Immersive Audio, Up to 15H Total Playback, Instant Voice Assistant and Type-C Charging,Bluetooth Earphone (Active Black)</t>
   </si>
   <si>
-    <t>Rs. 1,299</t>
+    <t>Rs. 1,499</t>
   </si>
   <si>
     <t>NBOX MARATHON Over Ear Bluetooth Neckband 20 Hours Playback IPX5(Splash &amp; Sweat Proof)BT 5.1 V Passive noise cancellation BLUETOOTH HEADPHONE -Bluetooth Silver</t>
@@ -26,16 +26,19 @@
     <t>Rs. 749</t>
   </si>
   <si>
+    <t>Truke Buds Q1 In Ear Bluetooth Earphone 8 Hours Playback Bluetooth IPX4(Splash Proof) Powerfull Bass -Bluetooth V 5.1 Black</t>
+  </si>
+  <si>
+    <t>Rs. 1,199</t>
+  </si>
+  <si>
     <t>NBOX Buzz TWS On Ear True Wireless (TWS) 20 Hours Playback IPX5(Splash &amp; Sweat Proof) Passive noise cancellation -Bluetooth Version 5.1 Black</t>
   </si>
   <si>
-    <t>boAt Airdopes 121v2 On Ear True Wireless (TWS) 14 Hours Playback IPX7(Water Resistant) Active Noise cancellation -Bluetooth V 5.0 Black</t>
+    <t>Syska HE5700 In Ear Bluetooth Neckband 6 Hours Playback IPX4(Splash &amp; Sweat Proof) Powerfull bass -Bluetooth V 5.0 Gray</t>
   </si>
   <si>
-    <t>Zebronics - Wireless Bluetooth Headset</t>
-  </si>
-  <si>
-    <t>Rs. 1,399</t>
+    <t>Rs. 899</t>
   </si>
 </sst>
 </file>
@@ -107,23 +110,23 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Parallel execution of Testclasses Dynamically
</commit_message>
<xml_diff>
--- a/ExcelFileData/WriteItemData.xlsx
+++ b/ExcelFileData/WriteItemData.xlsx
@@ -14,10 +14,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
-    <t>Varni Airgo In Ear Bluetooth Earphone Hours Playback Bluetooth IPX5(Splash Proof) Active Noise cancellation -Bluetooth White</t>
+    <t>VEhop GAMO, 24Hrs Play, 60ms Low Latency, On Ear Wireless With Mic Headphones/Earphones Black</t>
   </si>
   <si>
-    <t>Rs. 849</t>
+    <t>Rs. 1,199</t>
+  </si>
+  <si>
+    <t>pTron Bassbuds Sports On Ear Bluetooth Headphone 48 Hours Playback IPX4(Splash &amp; Sweat Proof) Passive noise cancellation -Bluetooth V 5.2 Black</t>
+  </si>
+  <si>
+    <t>Rs. 999</t>
   </si>
   <si>
     <t>boAt Airdopes 131/138 Twin Wireless Earbuds with IWP Technology, Bluetooth V5.0, Immersive Audio, Up to 15H Total Playback, Instant Voice Assistant and Type-C Charging,Bluetooth Earphone (Active Black)</t>
@@ -26,22 +32,16 @@
     <t>Rs. 1,499</t>
   </si>
   <si>
-    <t>Boult Audio Airbass X50 In Ear True Wireless (TWS) 40 Hours Playback IPX5(Splash &amp; Sweat Proof) Fast charging -Bluetooth White</t>
+    <t>Tecsox PowerHouse Earbud In Ear Bluetooth Earphone 45 Hours Playback Bluetooth IPX5(Splash Proof) Powerfull Bass -Bluetooth V 5.1 Black</t>
   </si>
   <si>
-    <t>Rs. 1,498</t>
+    <t>Rs. 725</t>
   </si>
   <si>
-    <t>boAt Rockerz 255 Pro Plus Neckband Wireless With Mic Headphones/Earphones(Blue)</t>
+    <t>Lenovo QE03 In Ear Bluetooth Neckband 8 Hours Playback IPX5(Splash &amp; Sweat Proof) Powerfull bass -Bluetooth V 5.0 Black</t>
   </si>
   <si>
-    <t>Rs. 1,599</t>
-  </si>
-  <si>
-    <t>Boult Audio Y1 In Ear True Wireless (TWS) 40 Hours Playback IPX5(Splash &amp; Sweat Proof) Powerfull bass -Bluetooth Black</t>
-  </si>
-  <si>
-    <t>Rs. 1,199</t>
+    <t>Rs. 899</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
ExecutionFlags Added for Dynamic Tests
</commit_message>
<xml_diff>
--- a/ExcelFileData/WriteItemData.xlsx
+++ b/ExcelFileData/WriteItemData.xlsx
@@ -12,24 +12,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
-    <t>VEhop GAMO, 24Hrs Play, 60ms Low Latency, On Ear Wireless With Mic Headphones/Earphones Black</t>
+    <t>Boult Audio AirBass z40 In Ear True Wireless (TWS) 60 Hours Playback IPX4(Splash &amp; Sweat Proof) Powerfull bass -Bluetooth White</t>
   </si>
   <si>
-    <t>Rs. 1,199</t>
+    <t>Rs. 1,499</t>
   </si>
   <si>
-    <t>pTron Bassbuds Sports On Ear Bluetooth Headphone 48 Hours Playback IPX4(Splash &amp; Sweat Proof) Passive noise cancellation -Bluetooth V 5.2 Black</t>
+    <t>NBOX Buzz TWS On Ear True Wireless (TWS) 20 Hours Playback IPX5(Splash &amp; Sweat Proof) Passive noise cancellation -Bluetooth Version 5.1 Black</t>
   </si>
   <si>
-    <t>Rs. 999</t>
+    <t>Rs. 745</t>
   </si>
   <si>
     <t>boAt Airdopes 131/138 Twin Wireless Earbuds with IWP Technology, Bluetooth V5.0, Immersive Audio, Up to 15H Total Playback, Instant Voice Assistant and Type-C Charging,Bluetooth Earphone (Active Black)</t>
-  </si>
-  <si>
-    <t>Rs. 1,499</t>
   </si>
   <si>
     <t>Tecsox PowerHouse Earbud In Ear Bluetooth Earphone 45 Hours Playback Bluetooth IPX5(Splash Proof) Powerfull Bass -Bluetooth V 5.1 Black</t>
@@ -38,10 +35,7 @@
     <t>Rs. 725</t>
   </si>
   <si>
-    <t>Lenovo QE03 In Ear Bluetooth Neckband 8 Hours Playback IPX5(Splash &amp; Sweat Proof) Powerfull bass -Bluetooth V 5.0 Black</t>
-  </si>
-  <si>
-    <t>Rs. 899</t>
+    <t>Boult Audio Airbass X50 In Ear True Wireless (TWS) 40 Hours Playback IPX5(Splash &amp; Sweat Proof) Fast charging -Bluetooth Black</t>
   </si>
 </sst>
 </file>
@@ -113,23 +107,23 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dynamic Browser provision added for custom TestNg
</commit_message>
<xml_diff>
--- a/ExcelFileData/WriteItemData.xlsx
+++ b/ExcelFileData/WriteItemData.xlsx
@@ -14,34 +14,34 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
-    <t>Varni Airgo In Ear Bluetooth Earphone Hours Playback Bluetooth IPX5(Splash Proof) Active Noise cancellation -Bluetooth White</t>
+    <t>Zebronics - Wireless Bluetooth Headset</t>
   </si>
   <si>
-    <t>Rs. 849</t>
+    <t>Rs. 1,449</t>
+  </si>
+  <si>
+    <t>BLUNT Air 1 Earbuds In Ear Bluetooth Earphone 6 Hours Playback Bluetooth IPX6(Water Resistant) Active Noise cancellation -Bluetooth V 5.1 Black</t>
+  </si>
+  <si>
+    <t>Rs. 1,299</t>
   </si>
   <si>
     <t>boAt Airdopes 131/138 Twin Wireless Earbuds with IWP Technology, Bluetooth V5.0, Immersive Audio, Up to 15H Total Playback, Instant Voice Assistant and Type-C Charging,Bluetooth Earphone (Active Black)</t>
   </si>
   <si>
-    <t>Rs. 1,499</t>
+    <t>Rs. 1,199</t>
   </si>
   <si>
-    <t>Boult Audio Airbass X50 In Ear True Wireless (TWS) 40 Hours Playback IPX5(Splash &amp; Sweat Proof) Fast charging -Bluetooth White</t>
+    <t>hitage TWS68 V5.0Earbuds In Ear True Wireless (TWS) 20 Hours Playback IPX4(Splash &amp; Sweat Proof) Comfirtable in ear fit -Bluetooth V 5.0 Red</t>
   </si>
   <si>
-    <t>Rs. 1,498</t>
+    <t>Rs. 795</t>
   </si>
   <si>
-    <t>boAt Rockerz 255 Pro Plus Neckband Wireless With Mic Headphones/Earphones(Blue)</t>
+    <t>Tecsox PowerHouse Earbud In Ear Bluetooth Earphone 45 Hours Playback Bluetooth IPX5(Splash Proof) Powerfull Bass -Bluetooth V 5.1 Black</t>
   </si>
   <si>
-    <t>Rs. 1,599</t>
-  </si>
-  <si>
-    <t>Boult Audio Y1 In Ear True Wireless (TWS) 40 Hours Playback IPX5(Splash &amp; Sweat Proof) Powerfull bass -Bluetooth Black</t>
-  </si>
-  <si>
-    <t>Rs. 1,199</t>
+    <t>Rs. 725</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
fixing chrome launching problem
</commit_message>
<xml_diff>
--- a/ExcelFileData/WriteItemData.xlsx
+++ b/ExcelFileData/WriteItemData.xlsx
@@ -14,34 +14,34 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
-    <t>Zebronics - Wireless Bluetooth Headset</t>
+    <t>Portronics - Wireless Bluetooth Headset</t>
   </si>
   <si>
-    <t>Rs. 1,449</t>
-  </si>
-  <si>
-    <t>BLUNT Air 1 Earbuds In Ear Bluetooth Earphone 6 Hours Playback Bluetooth IPX6(Water Resistant) Active Noise cancellation -Bluetooth V 5.1 Black</t>
-  </si>
-  <si>
-    <t>Rs. 1,299</t>
+    <t>Rs. 1,149</t>
   </si>
   <si>
     <t>boAt Airdopes 131/138 Twin Wireless Earbuds with IWP Technology, Bluetooth V5.0, Immersive Audio, Up to 15H Total Playback, Instant Voice Assistant and Type-C Charging,Bluetooth Earphone (Active Black)</t>
   </si>
   <si>
-    <t>Rs. 1,199</t>
-  </si>
-  <si>
-    <t>hitage TWS68 V5.0Earbuds In Ear True Wireless (TWS) 20 Hours Playback IPX4(Splash &amp; Sweat Proof) Comfirtable in ear fit -Bluetooth V 5.0 Red</t>
-  </si>
-  <si>
-    <t>Rs. 795</t>
+    <t>Rs. 1,499</t>
   </si>
   <si>
     <t>Tecsox PowerHouse Earbud In Ear Bluetooth Earphone 45 Hours Playback Bluetooth IPX5(Splash Proof) Powerfull Bass -Bluetooth V 5.1 Black</t>
   </si>
   <si>
     <t>Rs. 725</t>
+  </si>
+  <si>
+    <t>hitage NBT-6586+ Neckband In Ear Bluetooth Neckband 22 Hours Playback IPX6(Water Resistant) Fast charging -Bluetooth V 5.0 Red</t>
+  </si>
+  <si>
+    <t>Rs. 789</t>
+  </si>
+  <si>
+    <t>pTron Bassbuds Duo Ear Buds Wireless With Mic Headphones/Earphones White</t>
+  </si>
+  <si>
+    <t>Rs. 799</t>
   </si>
 </sst>
 </file>

</xml_diff>